<commit_message>
four new datasets requested
</commit_message>
<xml_diff>
--- a/correspondence_with_authors.xlsx
+++ b/correspondence_with_authors.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Documents/git_repos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Documents/git_repos/parkinsonsMetagenomicData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3B68D44-E893-F746-9854-5EFE1E6DFA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77A4BBD-2A7C-0C4A-B616-A9A739925EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36400" yWindow="320" windowWidth="28040" windowHeight="17440" xr2:uid="{71476288-B2DA-7943-BF64-C4DCB95989A5}"/>
+    <workbookView xWindow="30680" yWindow="-1960" windowWidth="30240" windowHeight="17520" xr2:uid="{71476288-B2DA-7943-BF64-C4DCB95989A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>time</t>
   </si>
@@ -53,9 +53,6 @@
     <t>email_Cc</t>
   </si>
   <si>
-    <t>object</t>
-  </si>
-  <si>
     <t>pedro.pereira@helsinki.fi; petri.auvinen@helsinki.fi</t>
   </si>
   <si>
@@ -77,12 +74,6 @@
     <t>5:32:00 PM (EST)</t>
   </si>
   <si>
-    <t>giacomo_email_user</t>
-  </si>
-  <si>
-    <t>personal</t>
-  </si>
-  <si>
     <t>QianY_2020</t>
   </si>
   <si>
@@ -96,6 +87,117 @@
   </si>
   <si>
     <t>5:29:00 PM (EST)</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>giacomo_email_used</t>
+  </si>
+  <si>
+    <t>email_body</t>
+  </si>
+  <si>
+    <t>Dear Dr. Finlay,
+I am writing on behalf of the Curated Metagenomic Data (cMD) project (Pasolli et al., 2017) led by prof Levi Waldron.
+We are currently working on a new data release focused on Parkinson’s disease in a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation.
+We appreciated reading your recent contribution in Movement Disorders (https://doi.org/10.1002/mds.29959) and for making the sequencing data publicly available. We would like to include your data set in our next cMD release. To do so, we would need have access to individual level metadata. The bare minimum is disease/health status, but age and sex are important as well.
+Ideally, it would be best if you could provide us with the full data set you worked with, both for the sake of completeness, reusability, and reproducibility of data, not to mention the higher visibility your contribution would gain.
+I am looking forward to discussing the details together.
+Best regards
+Giacomo Antonello, PhD</t>
+  </si>
+  <si>
+    <t>Dear Dr. Xiao,
+I am writing on behalf of the Curated Metagenomic Data (cMD) project (Pasolli et al., 2017) led by prof Levi Waldron.
+We are currently working on a new data release focused on Parkinson’s disease in a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation.
+We appreciated reading your contribution in Brain in 2020  (https://doi.org/10.1093/brain/awaa201) and for making the sequencing data publicly available. We would like to include your data set in our next cMD release. To do so, we would need have access to individual level metadata. The bare minimum is disease/health status, but age and sex are important as well.
+Ideally, it would be best if you could provide us with the full data set you worked with, both for the sake of completeness, reusability, and reproducibility of data, not to mention the higher visibility your contribution would gain.
+I am looking forward to discussing the details together.
+Best regards
+Giacomo Antonello, PhD</t>
+  </si>
+  <si>
+    <t>Dear Dr. Pereira,
+I am writing on behalf of the Curated Metagenomic Data (cMD) project (Pasolli et al., 2017) led by prof Levi Waldron.
+We are currently working on a new data release focused on Parkinson’s disease in a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation.
+We appreciated reading your contribution in Scientific Reports this year (https://doi.org/10.1038/s41598-024-69742-4) and for making the sequencing data publicly available. We would like to include your data set in our next cMD release. To do so, we would need have access to individual level metadata. The bare minimum is disease/health status, but age and sex are important as well.
+Ideally, it would be best if you could provide us with the full data set you worked with, both for the sake of completeness, reusability, and reproducibility of data, not to mention the higher visibility your contribution would gain.
+I am looking forward to discussing the details together.
+Best regards
+Giacomo Antonello, PhD</t>
+  </si>
+  <si>
+    <t>Dear professors Zhou and Wang,
+I am working on a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation to build a harmonized resource of all publicly available metagenomic data available for the study of the gut microbiome in Parkinson's disease. We are following the approach of the curatedMetagenomicData (cMD) initiative (Pasolli et al., 2017) to lower barriers to reuse and integrated analysis by the entire Parkinson's Disease research community to better understand the underlying causes of the disease
+To succeed, we need access to raw sequencing data and individual participant metadata, including the datasets you have generate in https://www.researchsquare.com/article/rs-11866/v2work and https://doi.org/10.3389/fmicb.2021.728479. We will uniformly process raw data through the latest version of bioBakery (https://huttenhower.sph.harvard.edu/biobakery_workflows/), and standardize participant data across all studies. The minimum data we need in order to include your study is the raw reads and Parkinson's disease/health status, but age and sex are important as well. Ideally, it would be best to share the full data set you worked with, for the sake of completeness, reusability, and reproducibility of results.
+I am confident you will understand the importance of this harmonization effort and will be part of it as a data contributor. I'm looking forward to discussing details, including addressing any limitations or concerns you have about data sharing.
+Giacomo Antonello, PhD
+Microbiome Analytics Core, ASAP Network
+MAC GitHub: https://github.com/ASAP-MAC
+Book a meeting with MAC: https://outlook.office365.com/book/ASAPMAC@CUNY907.onmicrosoft.com/</t>
+  </si>
+  <si>
+    <t>2:21:00 PM (EST)</t>
+  </si>
+  <si>
+    <t>Parkinson curatedMetagenomicData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZhangF_2020 </t>
+  </si>
+  <si>
+    <t>zyl609@hubu.edu.cn; wpq20110328@qq.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZhangF_2020; MaoL_2021 </t>
+  </si>
+  <si>
+    <t>NishiwakiH_2024</t>
+  </si>
+  <si>
+    <t>Dear all,
+I am working on a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation to build a harmonized resource of all publicly available metagenomic data available for the study of the gut microbiome in Parkinson's disease. We are following the approach of the curatedMetagenomicData (cMD) initiative (Pasolli et al., 2017) to lower barriers to reuse and integrated analysis by the entire Parkinson's Disease research community to better understand the underlying causes of the disease
+To succeed, we need access to raw sequencing data and individual participant metadata, including the datasets you have generated in https://www.nature.com/articles/s41531-024-00724-z. We will uniformly process raw data through the latest version of bioBakery (https://huttenhower.sph.harvard.edu/biobakery_workflows/), and standardize participant data across all studies. The minimum data we need in order to include your study is the raw reads and Parkinson's disease/health status, but age and sex are important as well. Ideally, it would be best to share the full data set you worked with, for the sake of completeness, reusability, and reproducibility of results.
+I am confident you will understand the importance of this harmonization effort and will be part of it as a data contributor. I'm looking forward to discussing details, including addressing any limitations or concerns you have about data sharing.
+Giacomo Antonello, PhD 
+Microbiome Analytics Core, ASAP Network
+MAC GitHub: https://github.com/ASAP-MAC
+Book a meeting with MAC: https://outlook.office365.com/book/ASAPMAC@CUNY907.onmicrosoft.com/</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>2:32:00 PM (EST)</t>
+  </si>
+  <si>
+    <t>hirasan@met.nagoya-u.ac.jp; ohnok@med.nagoya-u.ac.jp</t>
+  </si>
+  <si>
+    <t>Contribute to the parkinsonsCuratedMetagenomicsData</t>
+  </si>
+  <si>
+    <t>bork@EMBL-Heidelberg.de; wuellner@uni-bonn.de</t>
+  </si>
+  <si>
+    <t>BedarfJR_2017</t>
+  </si>
+  <si>
+    <t>2:45:00 PM (EST)</t>
+  </si>
+  <si>
+    <t>Dear professors Bork and Wüllner,
+I am working on a project funded by the "Aligning Science Across Parkinson" (ASAP) network and the Michael J. Fox foundation to build a harmonized resource of all publicly available metagenomic data available for the study of the gut microbiome in Parkinson's disease. We are following the approach of the curatedMetagenomicData (cMD) initiative (Pasolli et al., 2017) to lower barriers to reuse and integrated analysis by the entire Parkinson's Disease research community to better understand the underlying causes of the disease
+To succeed, we need access to raw sequencing data and individual participant metadata, including the datasets you have generated in https://genomemedicine.biomedcentral.com/articles/10.1186/s13073-017-0428-y. We will uniformly process raw data through the latest version of bioBakery (https://huttenhower.sph.harvard.edu/biobakery_workflows/), and standardize participant data across all studies. The minimum data we need in order to include your study is the raw reads and Parkinson's disease/health status, but age and sex are important as well. Ideally, it would be best to share the full data set you worked with, for the sake of completeness, reusability, and reproducibility of results.
+I am confident you will understand the importance of this harmonization effort and will be part of it as a data contributor. I'm looking forward to discussing details, including addressing any limitations or concerns you have about data sharing.
+Giacomo Antonello, PhD 
+Microbiome Analytics Core (MAC), ASAP Network
+MAC GitHub: https://github.com/ASAP-MAC
+Book a meeting with someone at MAC: https://outlook.office365.com/book/ASAPMAC@CUNY907.onmicrosoft.com/</t>
   </si>
 </sst>
 </file>
@@ -105,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,10 +224,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF1F2328"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,12 +289,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -490,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904FE74-FE71-AB42-82F8-064249236EAF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,101 +655,248 @@
     <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.5" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="404" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>45574</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="404" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>45573</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="404" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>45573</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>45574</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>45573</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>45573</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>45616</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>45616</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>45616</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45616</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -605,6 +905,12 @@
     <hyperlink ref="E2" r:id="rId3" xr:uid="{D82BB838-4C89-2B41-945F-A82C929747D9}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{1FA8B79E-A945-4747-A48F-660D54BA445B}"/>
     <hyperlink ref="E4" r:id="rId5" xr:uid="{8CACAD62-82E3-6043-9AAC-472DBAE150C0}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{13E31008-AD9B-7749-A785-7865EC782688}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{F0473209-23CB-9C41-897B-B926682FC2E8}"/>
+    <hyperlink ref="D7" r:id="rId8" display="hirasan@met.nagoya-u.ac.jp; " xr:uid="{9178BD29-E30A-7249-9581-42D5A03D34A1}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{FFFBA6DB-B057-7E42-AC71-B5ABCC11A724}"/>
+    <hyperlink ref="D8" r:id="rId10" display="bork@EMBL-Heidelberg.de;" xr:uid="{60BCAC60-6E7A-D643-9BB5-DDBF1E957F4A}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{9BC55545-236D-984F-BFC8-40B74DB00183}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>